<commit_message>
IO-fix completed: - feature: FxE is now independent from efficiency. - bug-fix: trd no longer appears in both FIO/FOE
</commit_message>
<xml_diff>
--- a/data/zenodo_ivan/_templates/template.xlsx
+++ b/data/zenodo_ivan/_templates/template.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ruiziv/switchdrive/ACCURACY/RESTORE/data_sources/zenodo_ivan/_templates/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ruiziv/switchdrive/ACCURACY/RESTORE/data/zenodo_ivan/_templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D95F0AAD-96D3-0145-A83C-DE4034EB5A24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AEC3395-7BF6-2644-AAF3-F1F3671FD893}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6380" yWindow="3300" windowWidth="26840" windowHeight="15940" xr2:uid="{C8E91F5A-09D8-B54C-89E0-1F786FBAF633}"/>
   </bookViews>
   <sheets>
     <sheet name="template" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>Name:</t>
   </si>
@@ -59,15 +59,9 @@
     <t>Parameter</t>
   </si>
   <si>
-    <t>Option</t>
-  </si>
-  <si>
     <t>Year</t>
   </si>
   <si>
-    <t>Period</t>
-  </si>
-  <si>
     <t>Value</t>
   </si>
   <si>
@@ -84,14 +78,25 @@
   </si>
   <si>
     <t>Note</t>
+  </si>
+  <si>
+    <t>Flow</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -119,8 +124,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -139,7 +145,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2013 - 2022">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -427,7 +433,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -435,25 +441,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C6B71EF-CC1C-7E48-8AB2-8A6FDFC8823F}">
-  <dimension ref="A1:M5"/>
+  <dimension ref="A1:L5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -461,45 +468,42 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D5" t="s">
-        <v>7</v>
-      </c>
-      <c r="E5" t="s">
+      <c r="E5" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="F5" t="s">
+      <c r="F5" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G5" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="G5" t="s">
+      <c r="H5" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="H5" t="s">
+      <c r="I5" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="I5" t="s">
+      <c r="J5" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="J5" t="s">
+      <c r="K5" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="K5" t="s">
+      <c r="L5" s="1" t="s">
         <v>14</v>
-      </c>
-      <c r="L5" t="s">
-        <v>15</v>
-      </c>
-      <c r="M5" t="s">
-        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>